<commit_message>
separate macroa analysis into one with labor market condition and the other with stock market. only export resutls needed.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/corrM.xlsx
+++ b/WorkingFolder/Tables/corrM.xlsx
@@ -489,49 +489,49 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.6897961103399451</v>
+        <v>-0.6954620276105178</v>
       </c>
       <c r="D2">
-        <v>-0.2035943559683977</v>
+        <v>-0.1880822818662423</v>
       </c>
       <c r="E2">
-        <v>0.07658550861757438</v>
+        <v>0.02914056319740949</v>
       </c>
       <c r="F2">
-        <v>-0.002045344272760061</v>
+        <v>0.03420913027474753</v>
       </c>
       <c r="G2">
-        <v>0.01290957909118949</v>
+        <v>0.05668549591695958</v>
       </c>
       <c r="H2">
-        <v>0.02004104860421435</v>
+        <v>0.08800201154955861</v>
       </c>
       <c r="J2">
-        <v>0.01936369248775929</v>
+        <v>0.1026585402629121</v>
       </c>
       <c r="K2">
-        <v>-0.05828071817647335</v>
+        <v>-0.09569731657107264</v>
       </c>
       <c r="L2">
-        <v>-0.1776113038751677</v>
+        <v>-0.15961449175092</v>
       </c>
       <c r="M2">
-        <v>0.0252683030334444</v>
+        <v>0.02671256140689233</v>
       </c>
       <c r="N2">
-        <v>0.05373952863575021</v>
+        <v>0.1245000835920851</v>
       </c>
       <c r="O2">
-        <v>-0.04572274689720179</v>
+        <v>0.02613467962342986</v>
       </c>
       <c r="P2">
-        <v>0.03751865469340517</v>
+        <v>0.1228681942988932</v>
       </c>
       <c r="Q2">
-        <v>-0.01295695864447187</v>
+        <v>-0.033236964184887</v>
       </c>
       <c r="R2">
-        <v>-0.03335443267855292</v>
+        <v>0.001600103591062275</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -539,52 +539,52 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.6897961103399451</v>
+        <v>-0.6954620276105178</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.1841687564732068</v>
+        <v>0.2748306532819472</v>
       </c>
       <c r="E3">
-        <v>-0.0453368031047253</v>
+        <v>-0.04857978195050124</v>
       </c>
       <c r="F3">
-        <v>0.01254328074079483</v>
+        <v>0.01255724259136151</v>
       </c>
       <c r="G3">
-        <v>0.03946359327769161</v>
+        <v>-0.01060018019543008</v>
       </c>
       <c r="H3">
-        <v>-0.07328817349843601</v>
+        <v>-0.1003275785479076</v>
       </c>
       <c r="J3">
-        <v>-0.06747201087674803</v>
+        <v>-0.09495840075131633</v>
       </c>
       <c r="K3">
-        <v>0.1117723134284229</v>
+        <v>0.1508618296685586</v>
       </c>
       <c r="L3">
-        <v>0.1231112757778762</v>
+        <v>0.09568134073151335</v>
       </c>
       <c r="M3">
-        <v>-0.05708090279091604</v>
+        <v>-0.08960471633066344</v>
       </c>
       <c r="N3">
-        <v>-0.04163833013386999</v>
+        <v>-0.1001432587328002</v>
       </c>
       <c r="O3">
-        <v>0.03307880574120719</v>
+        <v>0.01048147561741413</v>
       </c>
       <c r="P3">
-        <v>0.002891733744788976</v>
+        <v>-0.05947472534720946</v>
       </c>
       <c r="Q3">
-        <v>0.05069895762861504</v>
+        <v>0.07520151954958959</v>
       </c>
       <c r="R3">
-        <v>0.06532518096092371</v>
+        <v>0.06304668397542296</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -592,52 +592,52 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.2035943559683977</v>
+        <v>-0.1880822818662423</v>
       </c>
       <c r="C4">
-        <v>0.1841687564732068</v>
+        <v>0.2748306532819472</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>-0.5509569394695527</v>
+        <v>-0.5123597682070902</v>
       </c>
       <c r="F4">
-        <v>0.6293828400720779</v>
+        <v>0.5658061753654416</v>
       </c>
       <c r="G4">
-        <v>0.1223853848239987</v>
+        <v>0.1739951819953533</v>
       </c>
       <c r="H4">
-        <v>-0.1110244182334733</v>
+        <v>-0.2945441680967816</v>
       </c>
       <c r="J4">
-        <v>-0.1562932023579501</v>
+        <v>-0.2905985076269564</v>
       </c>
       <c r="K4">
-        <v>0.2891929810652991</v>
+        <v>0.3122181758795772</v>
       </c>
       <c r="L4">
-        <v>-0.2935209195746771</v>
+        <v>-0.2754181976148924</v>
       </c>
       <c r="M4">
-        <v>-0.1021273957489789</v>
+        <v>-0.03784677341782061</v>
       </c>
       <c r="N4">
-        <v>-0.3431864906725092</v>
+        <v>-0.32874929123365</v>
       </c>
       <c r="O4">
-        <v>-0.04354695927498966</v>
+        <v>0.06019978600222384</v>
       </c>
       <c r="P4">
-        <v>-0.2593700305742481</v>
+        <v>-0.2782325710945733</v>
       </c>
       <c r="Q4">
-        <v>0.2325284658972369</v>
+        <v>0.2684339346906659</v>
       </c>
       <c r="R4">
-        <v>-0.3325476846337796</v>
+        <v>-0.2432149506306212</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -645,52 +645,52 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.07658550861757438</v>
+        <v>0.02914056319740949</v>
       </c>
       <c r="C5">
-        <v>-0.0453368031047253</v>
+        <v>-0.04857978195050124</v>
       </c>
       <c r="D5">
-        <v>-0.5509569394695527</v>
+        <v>-0.5123597682070902</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>-0.8853663935137297</v>
+        <v>-0.8861524251917112</v>
       </c>
       <c r="G5">
-        <v>-0.2472242830355185</v>
+        <v>-0.3860168196198112</v>
       </c>
       <c r="H5">
-        <v>0.2455181015841376</v>
+        <v>0.488511382759929</v>
       </c>
       <c r="J5">
-        <v>0.2476947700305352</v>
+        <v>0.5327311332647087</v>
       </c>
       <c r="K5">
-        <v>-0.5071212350070473</v>
+        <v>-0.6725077643418644</v>
       </c>
       <c r="L5">
-        <v>0.5250884604087512</v>
+        <v>0.6935453139197432</v>
       </c>
       <c r="M5">
-        <v>0.0290179487843403</v>
+        <v>-0.09650071735825808</v>
       </c>
       <c r="N5">
-        <v>0.3857564457044987</v>
+        <v>0.5236914481283271</v>
       </c>
       <c r="O5">
-        <v>-0.01676470645845839</v>
+        <v>-0.2827997122318284</v>
       </c>
       <c r="P5">
-        <v>0.233130533751236</v>
+        <v>0.4559128407195984</v>
       </c>
       <c r="Q5">
-        <v>-0.4610320337244821</v>
+        <v>-0.6020672565082923</v>
       </c>
       <c r="R5">
-        <v>0.425742931537725</v>
+        <v>0.5893034284480509</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -698,52 +698,52 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-0.002045344272760061</v>
+        <v>0.03420913027474753</v>
       </c>
       <c r="C6">
-        <v>0.01254328074079483</v>
+        <v>0.01255724259136151</v>
       </c>
       <c r="D6">
-        <v>0.6293828400720779</v>
+        <v>0.5658061753654416</v>
       </c>
       <c r="E6">
-        <v>-0.8853663935137297</v>
+        <v>-0.8861524251917112</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.2461524043334889</v>
+        <v>0.3335582946014879</v>
       </c>
       <c r="H6">
-        <v>-0.2573280506804081</v>
+        <v>-0.5229843227986096</v>
       </c>
       <c r="J6">
-        <v>-0.2878351454495143</v>
+        <v>-0.5422989646417723</v>
       </c>
       <c r="K6">
-        <v>0.3335690869735569</v>
+        <v>0.4056758208164513</v>
       </c>
       <c r="L6">
-        <v>-0.5305236742909295</v>
+        <v>-0.6304082599202043</v>
       </c>
       <c r="M6">
-        <v>-0.0722913944078757</v>
+        <v>-0.001045408961199361</v>
       </c>
       <c r="N6">
-        <v>-0.4363268788593173</v>
+        <v>-0.5212886093024264</v>
       </c>
       <c r="O6">
-        <v>0.02368371637615231</v>
+        <v>0.270433041677948</v>
       </c>
       <c r="P6">
-        <v>-0.288938292099288</v>
+        <v>-0.446859052656183</v>
       </c>
       <c r="Q6">
-        <v>0.2981308511155079</v>
+        <v>0.3654188162483002</v>
       </c>
       <c r="R6">
-        <v>-0.3980216784125754</v>
+        <v>-0.4870047038530387</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -751,52 +751,52 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.01290957909118949</v>
+        <v>0.05668549591695958</v>
       </c>
       <c r="C7">
-        <v>0.03946359327769161</v>
+        <v>-0.01060018019543008</v>
       </c>
       <c r="D7">
-        <v>0.1223853848239987</v>
+        <v>0.1739951819953533</v>
       </c>
       <c r="E7">
-        <v>-0.2472242830355185</v>
+        <v>-0.3860168196198112</v>
       </c>
       <c r="F7">
-        <v>0.2461524043334889</v>
+        <v>0.3335582946014879</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.3242574197365707</v>
+        <v>0.2282144331985945</v>
       </c>
       <c r="J7">
-        <v>0.2995101764734562</v>
+        <v>0.2017522194473726</v>
       </c>
       <c r="K7">
-        <v>0.3955375268173798</v>
+        <v>0.3703485431360334</v>
       </c>
       <c r="L7">
-        <v>-0.0132976252817473</v>
+        <v>-0.07823792394983131</v>
       </c>
       <c r="M7">
-        <v>0.7992225413587013</v>
+        <v>0.813853831783909</v>
       </c>
       <c r="N7">
-        <v>0.1213210703991177</v>
+        <v>0.1591991380261942</v>
       </c>
       <c r="O7">
-        <v>0.007483317921326854</v>
+        <v>-0.1978194138819634</v>
       </c>
       <c r="P7">
-        <v>0.04365159251840433</v>
+        <v>0.1469122152520484</v>
       </c>
       <c r="Q7">
-        <v>0.3678978502472589</v>
+        <v>0.3630575348992239</v>
       </c>
       <c r="R7">
-        <v>0.008796204539160919</v>
+        <v>-0.07265664635526758</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -804,52 +804,52 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.02004104860421435</v>
+        <v>0.08800201154955861</v>
       </c>
       <c r="C8">
-        <v>-0.07328817349843601</v>
+        <v>-0.1003275785479076</v>
       </c>
       <c r="D8">
-        <v>-0.1110244182334733</v>
+        <v>-0.2945441680967816</v>
       </c>
       <c r="E8">
-        <v>0.2455181015841376</v>
+        <v>0.488511382759929</v>
       </c>
       <c r="F8">
-        <v>-0.2573280506804081</v>
+        <v>-0.5229843227986096</v>
       </c>
       <c r="G8">
-        <v>0.3242574197365707</v>
+        <v>0.2282144331985945</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0.9593367903415715</v>
+        <v>0.9792641151560048</v>
       </c>
       <c r="K8">
-        <v>0.3312575750638658</v>
+        <v>-0.05211753778901478</v>
       </c>
       <c r="L8">
-        <v>0.3298054067286034</v>
+        <v>0.6829028338744026</v>
       </c>
       <c r="M8">
-        <v>0.609254790913381</v>
+        <v>0.48402467427776</v>
       </c>
       <c r="N8">
-        <v>0.09070312376154253</v>
+        <v>0.7269516643205035</v>
       </c>
       <c r="O8">
-        <v>-0.0625639460328196</v>
+        <v>-0.2839099923732194</v>
       </c>
       <c r="P8">
-        <v>-0.1674921320028981</v>
+        <v>0.6208983952960462</v>
       </c>
       <c r="Q8">
-        <v>0.3506151995279669</v>
+        <v>0.04958524081280442</v>
       </c>
       <c r="R8">
-        <v>0.0980603607745419</v>
+        <v>0.527323953863141</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -862,52 +862,52 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.01936369248775929</v>
+        <v>0.1026585402629121</v>
       </c>
       <c r="C10">
-        <v>-0.06747201087674803</v>
+        <v>-0.09495840075131633</v>
       </c>
       <c r="D10">
-        <v>-0.1562932023579501</v>
+        <v>-0.2905985076269564</v>
       </c>
       <c r="E10">
-        <v>0.2476947700305352</v>
+        <v>0.5327311332647087</v>
       </c>
       <c r="F10">
-        <v>-0.2878351454495143</v>
+        <v>-0.5422989646417723</v>
       </c>
       <c r="G10">
-        <v>0.2995101764734562</v>
+        <v>0.2017522194473726</v>
       </c>
       <c r="H10">
-        <v>0.9593367903415715</v>
+        <v>0.9792641151560048</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.281471712204577</v>
+        <v>-0.09840861227319085</v>
       </c>
       <c r="L10">
-        <v>0.378371683812899</v>
+        <v>0.7164471536491567</v>
       </c>
       <c r="M10">
-        <v>0.5761133745697244</v>
+        <v>0.4649076623324462</v>
       </c>
       <c r="N10">
-        <v>0.187578055402155</v>
+        <v>0.7604571890318254</v>
       </c>
       <c r="O10">
-        <v>-0.01825362543462824</v>
+        <v>-0.2806547402725821</v>
       </c>
       <c r="P10">
-        <v>-0.06572616774404921</v>
+        <v>0.6602733475555668</v>
       </c>
       <c r="Q10">
-        <v>0.3201275896166049</v>
+        <v>0.007045408321917977</v>
       </c>
       <c r="R10">
-        <v>0.1481057486721723</v>
+        <v>0.5855897097062018</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -915,52 +915,52 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.05828071817647335</v>
+        <v>-0.09569731657107264</v>
       </c>
       <c r="C11">
-        <v>0.1117723134284229</v>
+        <v>0.1508618296685586</v>
       </c>
       <c r="D11">
-        <v>0.2891929810652991</v>
+        <v>0.3122181758795772</v>
       </c>
       <c r="E11">
-        <v>-0.5071212350070473</v>
+        <v>-0.6725077643418644</v>
       </c>
       <c r="F11">
-        <v>0.3335690869735569</v>
+        <v>0.4056758208164513</v>
       </c>
       <c r="G11">
-        <v>0.3955375268173798</v>
+        <v>0.3703485431360334</v>
       </c>
       <c r="H11">
-        <v>0.3312575750638658</v>
+        <v>-0.05211753778901478</v>
       </c>
       <c r="J11">
-        <v>0.281471712204577</v>
+        <v>-0.09840861227319085</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>-0.226994598066938</v>
+        <v>-0.2857460969514533</v>
       </c>
       <c r="M11">
-        <v>0.4133306079946346</v>
+        <v>0.3130512932906556</v>
       </c>
       <c r="N11">
-        <v>-0.1548652599095349</v>
+        <v>-0.06611384108455527</v>
       </c>
       <c r="O11">
-        <v>-0.2846512465783188</v>
+        <v>0.03376595019548962</v>
       </c>
       <c r="P11">
-        <v>-0.2176722032077225</v>
+        <v>-0.05246523971468067</v>
       </c>
       <c r="Q11">
-        <v>0.8968577983671087</v>
+        <v>0.8799916556406883</v>
       </c>
       <c r="R11">
-        <v>-0.1785815821272974</v>
+        <v>-0.2643290939009635</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -968,52 +968,52 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.1776113038751677</v>
+        <v>-0.15961449175092</v>
       </c>
       <c r="C12">
-        <v>0.1231112757778762</v>
+        <v>0.09568134073151335</v>
       </c>
       <c r="D12">
-        <v>-0.2935209195746771</v>
+        <v>-0.2754181976148924</v>
       </c>
       <c r="E12">
-        <v>0.5250884604087512</v>
+        <v>0.6935453139197432</v>
       </c>
       <c r="F12">
-        <v>-0.5305236742909295</v>
+        <v>-0.6304082599202043</v>
       </c>
       <c r="G12">
-        <v>-0.0132976252817473</v>
+        <v>-0.07823792394983131</v>
       </c>
       <c r="H12">
-        <v>0.3298054067286034</v>
+        <v>0.6829028338744026</v>
       </c>
       <c r="J12">
-        <v>0.378371683812899</v>
+        <v>0.7164471536491567</v>
       </c>
       <c r="K12">
-        <v>-0.226994598066938</v>
+        <v>-0.2857460969514533</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.1552746577572451</v>
+        <v>0.2144274027338346</v>
       </c>
       <c r="N12">
-        <v>0.6253826188684255</v>
+        <v>0.6813215027964721</v>
       </c>
       <c r="O12">
-        <v>0.07452806790010968</v>
+        <v>-0.3284431669736942</v>
       </c>
       <c r="P12">
-        <v>0.4723374501919353</v>
+        <v>0.6005636968464753</v>
       </c>
       <c r="Q12">
-        <v>-0.219600254447085</v>
+        <v>-0.2324013050705599</v>
       </c>
       <c r="R12">
-        <v>0.7368945740904715</v>
+        <v>0.8191268319089997</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1021,52 +1021,52 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.0252683030334444</v>
+        <v>0.02671256140689233</v>
       </c>
       <c r="C13">
-        <v>-0.05708090279091604</v>
+        <v>-0.08960471633066344</v>
       </c>
       <c r="D13">
-        <v>-0.1021273957489789</v>
+        <v>-0.03784677341782061</v>
       </c>
       <c r="E13">
-        <v>0.0290179487843403</v>
+        <v>-0.09650071735825808</v>
       </c>
       <c r="F13">
-        <v>-0.0722913944078757</v>
+        <v>-0.001045408961199361</v>
       </c>
       <c r="G13">
-        <v>0.7992225413587013</v>
+        <v>0.813853831783909</v>
       </c>
       <c r="H13">
-        <v>0.609254790913381</v>
+        <v>0.48402467427776</v>
       </c>
       <c r="J13">
-        <v>0.5761133745697244</v>
+        <v>0.4649076623324462</v>
       </c>
       <c r="K13">
-        <v>0.4133306079946346</v>
+        <v>0.3130512932906556</v>
       </c>
       <c r="L13">
-        <v>0.1552746577572451</v>
+        <v>0.2144274027338346</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.266704296782332</v>
+        <v>0.4559212458883087</v>
       </c>
       <c r="O13">
-        <v>-0.06402039008662685</v>
+        <v>-0.234262498405988</v>
       </c>
       <c r="P13">
-        <v>0.07576955054845577</v>
+        <v>0.3802176799489076</v>
       </c>
       <c r="Q13">
-        <v>0.4751217281760241</v>
+        <v>0.3946292024424908</v>
       </c>
       <c r="R13">
-        <v>0.1600804616133711</v>
+        <v>0.1383314059606824</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1074,52 +1074,52 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.05373952863575021</v>
+        <v>0.1245000835920851</v>
       </c>
       <c r="C14">
-        <v>-0.04163833013386999</v>
+        <v>-0.1001432587328002</v>
       </c>
       <c r="D14">
-        <v>-0.3431864906725092</v>
+        <v>-0.32874929123365</v>
       </c>
       <c r="E14">
-        <v>0.3857564457044987</v>
+        <v>0.5236914481283271</v>
       </c>
       <c r="F14">
-        <v>-0.4363268788593173</v>
+        <v>-0.5212886093024264</v>
       </c>
       <c r="G14">
-        <v>0.1213210703991177</v>
+        <v>0.1591991380261942</v>
       </c>
       <c r="H14">
-        <v>0.09070312376154253</v>
+        <v>0.7269516643205035</v>
       </c>
       <c r="J14">
-        <v>0.187578055402155</v>
+        <v>0.7604571890318254</v>
       </c>
       <c r="K14">
-        <v>-0.1548652599095349</v>
+        <v>-0.06611384108455527</v>
       </c>
       <c r="L14">
-        <v>0.6253826188684255</v>
+        <v>0.6813215027964721</v>
       </c>
       <c r="M14">
-        <v>0.266704296782332</v>
+        <v>0.4559212458883087</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0.1105593263013635</v>
+        <v>-0.3963776518294763</v>
       </c>
       <c r="P14">
-        <v>0.9361045980913972</v>
+        <v>0.9672529628894712</v>
       </c>
       <c r="Q14">
-        <v>-0.1065908832214402</v>
+        <v>0.01228289385372508</v>
       </c>
       <c r="R14">
-        <v>0.7273332791172671</v>
+        <v>0.7649321850275498</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1127,52 +1127,52 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.04572274689720179</v>
+        <v>0.02613467962342986</v>
       </c>
       <c r="C15">
-        <v>0.03307880574120719</v>
+        <v>0.01048147561741413</v>
       </c>
       <c r="D15">
-        <v>-0.04354695927498966</v>
+        <v>0.06019978600222384</v>
       </c>
       <c r="E15">
-        <v>-0.01676470645845839</v>
+        <v>-0.2827997122318284</v>
       </c>
       <c r="F15">
-        <v>0.02368371637615231</v>
+        <v>0.270433041677948</v>
       </c>
       <c r="G15">
-        <v>0.007483317921326854</v>
+        <v>-0.1978194138819634</v>
       </c>
       <c r="H15">
-        <v>-0.0625639460328196</v>
+        <v>-0.2839099923732194</v>
       </c>
       <c r="J15">
-        <v>-0.01825362543462824</v>
+        <v>-0.2806547402725821</v>
       </c>
       <c r="K15">
-        <v>-0.2846512465783188</v>
+        <v>0.03376595019548962</v>
       </c>
       <c r="L15">
-        <v>0.07452806790010968</v>
+        <v>-0.3284431669736942</v>
       </c>
       <c r="M15">
-        <v>-0.06402039008662685</v>
+        <v>-0.234262498405988</v>
       </c>
       <c r="N15">
-        <v>0.1105593263013635</v>
+        <v>-0.3963776518294763</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15">
-        <v>0.1154152913399076</v>
+        <v>-0.3679922888892923</v>
       </c>
       <c r="Q15">
-        <v>-0.2035253583151278</v>
+        <v>0.03262038920980954</v>
       </c>
       <c r="R15">
-        <v>-0.04743242383832395</v>
+        <v>-0.3029930305327576</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1180,52 +1180,52 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.03751865469340517</v>
+        <v>0.1228681942988932</v>
       </c>
       <c r="C16">
-        <v>0.002891733744788976</v>
+        <v>-0.05947472534720946</v>
       </c>
       <c r="D16">
-        <v>-0.2593700305742481</v>
+        <v>-0.2782325710945733</v>
       </c>
       <c r="E16">
-        <v>0.233130533751236</v>
+        <v>0.4559128407195984</v>
       </c>
       <c r="F16">
-        <v>-0.288938292099288</v>
+        <v>-0.446859052656183</v>
       </c>
       <c r="G16">
-        <v>0.04365159251840433</v>
+        <v>0.1469122152520484</v>
       </c>
       <c r="H16">
-        <v>-0.1674921320028981</v>
+        <v>0.6208983952960462</v>
       </c>
       <c r="J16">
-        <v>-0.06572616774404921</v>
+        <v>0.6602733475555668</v>
       </c>
       <c r="K16">
-        <v>-0.2176722032077225</v>
+        <v>-0.05246523971468067</v>
       </c>
       <c r="L16">
-        <v>0.4723374501919353</v>
+        <v>0.6005636968464753</v>
       </c>
       <c r="M16">
-        <v>0.07576955054845577</v>
+        <v>0.3802176799489076</v>
       </c>
       <c r="N16">
-        <v>0.9361045980913972</v>
+        <v>0.9672529628894712</v>
       </c>
       <c r="O16">
-        <v>0.1154152913399076</v>
+        <v>-0.3679922888892923</v>
       </c>
       <c r="P16">
         <v>1</v>
       </c>
       <c r="Q16">
-        <v>-0.1836060800839042</v>
+        <v>-0.006289716343228092</v>
       </c>
       <c r="R16">
-        <v>0.6826277671728377</v>
+        <v>0.7638521715591707</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1233,52 +1233,52 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.01295695864447187</v>
+        <v>-0.033236964184887</v>
       </c>
       <c r="C17">
-        <v>0.05069895762861504</v>
+        <v>0.07520151954958959</v>
       </c>
       <c r="D17">
-        <v>0.2325284658972369</v>
+        <v>0.2684339346906659</v>
       </c>
       <c r="E17">
-        <v>-0.4610320337244821</v>
+        <v>-0.6020672565082923</v>
       </c>
       <c r="F17">
-        <v>0.2981308511155079</v>
+        <v>0.3654188162483002</v>
       </c>
       <c r="G17">
-        <v>0.3678978502472589</v>
+        <v>0.3630575348992239</v>
       </c>
       <c r="H17">
-        <v>0.3506151995279669</v>
+        <v>0.04958524081280442</v>
       </c>
       <c r="J17">
-        <v>0.3201275896166049</v>
+        <v>0.007045408321917977</v>
       </c>
       <c r="K17">
-        <v>0.8968577983671087</v>
+        <v>0.8799916556406883</v>
       </c>
       <c r="L17">
-        <v>-0.219600254447085</v>
+        <v>-0.2324013050705599</v>
       </c>
       <c r="M17">
-        <v>0.4751217281760241</v>
+        <v>0.3946292024424908</v>
       </c>
       <c r="N17">
-        <v>-0.1065908832214402</v>
+        <v>0.01228289385372508</v>
       </c>
       <c r="O17">
-        <v>-0.2035253583151278</v>
+        <v>0.03262038920980954</v>
       </c>
       <c r="P17">
-        <v>-0.1836060800839042</v>
+        <v>-0.006289716343228092</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
       <c r="R17">
-        <v>-0.2073451894415046</v>
+        <v>-0.2590281121190497</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1286,49 +1286,49 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.03335443267855292</v>
+        <v>0.001600103591062275</v>
       </c>
       <c r="C18">
-        <v>0.06532518096092371</v>
+        <v>0.06304668397542296</v>
       </c>
       <c r="D18">
-        <v>-0.3325476846337796</v>
+        <v>-0.2432149506306212</v>
       </c>
       <c r="E18">
-        <v>0.425742931537725</v>
+        <v>0.5893034284480509</v>
       </c>
       <c r="F18">
-        <v>-0.3980216784125754</v>
+        <v>-0.4870047038530387</v>
       </c>
       <c r="G18">
-        <v>0.008796204539160919</v>
+        <v>-0.07265664635526758</v>
       </c>
       <c r="H18">
-        <v>0.0980603607745419</v>
+        <v>0.527323953863141</v>
       </c>
       <c r="J18">
-        <v>0.1481057486721723</v>
+        <v>0.5855897097062018</v>
       </c>
       <c r="K18">
-        <v>-0.1785815821272974</v>
+        <v>-0.2643290939009635</v>
       </c>
       <c r="L18">
-        <v>0.7368945740904715</v>
+        <v>0.8191268319089997</v>
       </c>
       <c r="M18">
-        <v>0.1600804616133711</v>
+        <v>0.1383314059606824</v>
       </c>
       <c r="N18">
-        <v>0.7273332791172671</v>
+        <v>0.7649321850275498</v>
       </c>
       <c r="O18">
-        <v>-0.04743242383832395</v>
+        <v>-0.3029930305327576</v>
       </c>
       <c r="P18">
-        <v>0.6826277671728377</v>
+        <v>0.7638521715591707</v>
       </c>
       <c r="Q18">
-        <v>-0.2073451894415046</v>
+        <v>-0.2590281121190497</v>
       </c>
       <c r="R18">
         <v>1</v>

</xml_diff>